<commit_message>
Alterado para tabela real de alunos
</commit_message>
<xml_diff>
--- a/CST_EDA_2025.xlsx
+++ b/CST_EDA_2025.xlsx
@@ -46,52 +46,52 @@
     <t xml:space="preserve">Recuperação 03</t>
   </si>
   <si>
-    <t xml:space="preserve">LUCAS MENEZES DOS SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRENDA LIMA COSTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FELIPE HENRIQUE FERREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUSTAVO RAMOS NOGUEIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HENRIQUE CARDOSO LEAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISABELLA SOUZA FARIAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VINICIUS SANTANA LOPES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAURA VIEIRA ALMEIDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DANIELA RIBEIRO MORAES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TATIANA LOPES BARBOSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDUARDO CASTRO TEIXEIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROBERTO GOMES BASTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANUELA DIAS MOREIRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIEGO COSTA BRAGA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAYANE OLIVEIRA PIRES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THIAGO FREITAS CAVALCANTE</t>
+    <t xml:space="preserve">ARTHUR MAZZARDO NAUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS ALBERTO DE SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DANIEL DIFENTTHAELER SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABRIEL LAZZARI OLIVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GABRIEL MENDES ALVES ORTIZ PAULO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGOR RODRIGUES ESTEVÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOAO PEDRO CARDOSO PERFEITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUIZ FELIPE SCHALATA PACHECO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA EDUARDA DE OLIVEIRA ALVES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARILIA STEFENON RODRIGUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICHEL DAVID DE SOUZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSWALDO GABRIEL CARDOSO CORRÊA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATRICIA VOIGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDRO JAREMCZUK ZANONI SILVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RODRIGO RAMOS DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VICTOR LEONARDO FAGUNDES DOS SANTOS</t>
   </si>
 </sst>
 </file>
@@ -310,7 +310,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,7 +356,7 @@
       <c r="A2" s="3" t="n">
         <v>202410004440</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="n">
@@ -370,7 +370,7 @@
       <c r="A3" s="3" t="n">
         <v>202310003436</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -390,7 +390,7 @@
       <c r="A4" s="3" t="n">
         <v>202410003560</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="n">
@@ -404,7 +404,7 @@
       <c r="A5" s="3" t="n">
         <v>202410000490</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -424,7 +424,7 @@
       <c r="A6" s="3" t="n">
         <v>202410004424</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
@@ -444,7 +444,7 @@
       <c r="A7" s="3" t="n">
         <v>202410003584</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="n">
@@ -464,7 +464,7 @@
       <c r="A8" s="3" t="n">
         <v>202410003931</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="n">
@@ -478,7 +478,7 @@
       <c r="A9" s="3" t="n">
         <v>202410005122</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="n">
@@ -498,7 +498,7 @@
       <c r="A10" s="3" t="n">
         <v>202310007170</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="n">
@@ -518,7 +518,7 @@
       <c r="A11" s="3" t="n">
         <v>202310023418</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="n">
@@ -538,7 +538,7 @@
       <c r="A12" s="3" t="n">
         <v>202410003937</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="n">
@@ -558,7 +558,7 @@
       <c r="A13" s="3" t="n">
         <v>202410050430</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="n">
@@ -572,7 +572,7 @@
       <c r="A14" s="3" t="n">
         <v>202410008932</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="n">
@@ -592,7 +592,7 @@
       <c r="A15" s="3" t="n">
         <v>202410003510</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -600,7 +600,7 @@
       <c r="A16" s="3" t="n">
         <v>202410003233</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="n">
@@ -614,7 +614,7 @@
       <c r="A17" s="3" t="n">
         <v>202410009226</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="n">

</xml_diff>